<commit_message>
fixed and merged  health insurance and initial consultation
</commit_message>
<xml_diff>
--- a/mapping/mml_first_clinic_mapping.xlsx
+++ b/mapping/mml_first_clinic_mapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="227">
   <si>
     <t>Archetype</t>
     <phoneticPr fontId="1"/>
@@ -313,10 +313,6 @@
     <t>mmlFc:name</t>
   </si>
   <si>
-    <t>Name of organization</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>mmlFc:repCode</t>
   </si>
   <si>
@@ -360,10 +356,6 @@
     <t>MML0001</t>
   </si>
   <si>
-    <t>Identifier chedi digit schema</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>openEHR-EHR-EVALUATION.family_history.v1</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -444,10 +436,6 @@
   </si>
   <si>
     <t>openEHR-EHR-EVALUATION.vaccination_summary-mml.v1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Infection Diseases or Agent</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -543,18 +531,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/content[openEHR-EHR-EVALUATION.family_history.v1 and name/value='Family history']/data[at0001]/items[at0003 and name/value='Per family member']/items[at0008 and name/value='Medical history']/items[at0009]/term_mappings[1]/defining_code/code_string</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-EVALUATION.family_history.v1 and name/value='Family history']/data[at0001]/items[at0003 and name/value='Per family member']/items[at0008 and name/value='Medical history']/items[at0009]/term_mappings[1]/defining_code/terminology_id/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-EVALUATION.family_history.v1 and name/value='Family history']/data[at0001]/items[at0003 and name/value='Per family member']/items[at0008 and name/value='Medical history']/items[at0009]/term_mappings[1]/match</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>*値は"="で固定</t>
     <rPh sb="1" eb="2">
       <t>アタイ</t>
@@ -605,18 +581,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/content[openEHR-EHR-SECTION.adhoc.v1 and name/value='childhood']/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='birth info']/items[openEHR-EHR-OBSERVATION.birth.v1 and name/value='Birth record for MML']/data[at0001]/events[at0002]/data[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Facility']/items[at0.12]/term_mappings[1]/defining_code/code_string</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-SECTION.adhoc.v1 and name/value='childhood']/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='birth info']/items[openEHR-EHR-OBSERVATION.birth.v1 and name/value='Birth record for MML']/data[at0001]/events[at0002]/data[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Facility']/items[at0.12]/term_mappings/defining_code/terminology_id/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-SECTION.adhoc.v1 and name/value='childhood']/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='birth info']/items[openEHR-EHR-OBSERVATION.birth.v1 and name/value='Birth record for MML']/data[at0001]/events[at0002]/data[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Facility']/items[at0.12]/term_mappings/match</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>DV_QUANTITY</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -697,10 +661,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>infections disease or agent</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>comment</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -810,6 +770,72 @@
   </si>
   <si>
     <t>Relationship</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlRd:uid</t>
+  </si>
+  <si>
+    <t>Name of organisation</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Identifier check digit schema</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Infectious Disease or agent</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Infectious Disease or Agent</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>node</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>data type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>openEHR-EHR-CLUSTER.free_text.v1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FreeText</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DV_TEXT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/context/other_context[at0001]/items[openEHR-EHR-CLUSTER.free_text.v1 and name/value='Health insurance']/items[at0001 and name/value='related uid']</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.adhoc.v1 and name/value='childhood']/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='birth info']/items[openEHR-EHR-OBSERVATION.birth.v1 and name/value='Birth record for MML']/data[at0001]/events[at0002]/data[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Facility']/items[at0.12]/mappings/target/defining_code/code_string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.adhoc.v1 and name/value='childhood']/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='birth info']/items[openEHR-EHR-OBSERVATION.birth.v1 and name/value='Birth record for MML']/data[at0001]/events[at0002]/data[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Facility']/items[at0.12]/mappings/target/defining_code/terminology_id/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.adhoc.v1 and name/value='childhood']/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='birth info']/items[openEHR-EHR-OBSERVATION.birth.v1 and name/value='Birth record for MML']/data[at0001]/events[at0002]/data[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Facility']/items[at0.12]/mappings/match</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-EVALUATION.family_history.v1 and name/value='Family history']/data[at0001]/items[at0003 and name/value='Per family member']/items[at0008 and name/value='Medical history']/items[at0009]/mappings/target/defining_code/code_string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-EVALUATION.family_history.v1 and name/value='Family history']/data[at0001]/items[at0003 and name/value='Per family member']/items[at0008 and name/value='Medical history']/items[at0009]/mappings/target/defining_code/terminology_id/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-EVALUATION.family_history.v1 and name/value='Family history']/data[at0001]/items[at0003 and name/value='Per family member']/items[at0008 and name/value='Medical history']/items[at0009]/mappings/match</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -842,7 +868,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -858,6 +884,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -906,7 +938,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -942,6 +974,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1244,10 +1288,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L68"/>
+  <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="C35" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="L69" sqref="L69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1279,6 +1323,12 @@
       <c r="I2" t="s">
         <v>13</v>
       </c>
+      <c r="J2" t="s">
+        <v>215</v>
+      </c>
+      <c r="K2" t="s">
+        <v>216</v>
+      </c>
       <c r="L2" t="s">
         <v>1</v>
       </c>
@@ -1328,7 +1378,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="H5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.15">
@@ -1361,16 +1411,16 @@
         <v>29</v>
       </c>
       <c r="I7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J7" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="K7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="L7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.15">
@@ -1397,16 +1447,16 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="I9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J9" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="K9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.15">
@@ -1423,10 +1473,10 @@
       </c>
       <c r="F10" s="3"/>
       <c r="I10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L10" t="s">
-        <v>154</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
@@ -1443,7 +1493,7 @@
       </c>
       <c r="F11" s="3"/>
       <c r="L11" t="s">
-        <v>155</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
@@ -1454,10 +1504,10 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="H12" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="L12" t="s">
-        <v>156</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
@@ -1537,7 +1587,7 @@
       </c>
       <c r="F18" s="9"/>
       <c r="I18" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.15">
@@ -1641,7 +1691,9 @@
       <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A25" s="9"/>
+      <c r="A25" s="9">
+        <v>1</v>
+      </c>
       <c r="B25" s="9" t="s">
         <v>92</v>
       </c>
@@ -1652,82 +1704,94 @@
       </c>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A26" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="3"/>
-      <c r="I26" t="s">
-        <v>114</v>
-      </c>
-      <c r="J26" t="s">
+    <row r="26" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="H26" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="K26" t="s">
-        <v>158</v>
-      </c>
-      <c r="L26" t="s">
-        <v>159</v>
+      <c r="J26" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="3"/>
       <c r="I27" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J27" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="K27" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="L27" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F28" s="3"/>
+      <c r="I28" t="s">
+        <v>113</v>
+      </c>
+      <c r="J28" t="s">
+        <v>194</v>
+      </c>
+      <c r="K28" t="s">
+        <v>147</v>
+      </c>
+      <c r="L28" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1738,150 +1802,137 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="E30" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="F30" s="3"/>
-      <c r="H30" t="s">
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A31" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="H31" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="3"/>
-      <c r="I31" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="K31" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="L31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3" t="s">
-        <v>97</v>
-      </c>
+      <c r="B32" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>162</v>
+        <v>15</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="I32" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="L32" t="s">
-        <v>163</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F33" s="3"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
+        <v>45</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>156</v>
+      </c>
       <c r="L33" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
-      <c r="B34" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="D34" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="F34" s="3"/>
-      <c r="I34" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="K34" s="5" t="s">
-        <v>165</v>
-      </c>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
       <c r="L34" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
-      <c r="C35" s="3" t="s">
-        <v>102</v>
-      </c>
+      <c r="B35" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>167</v>
+        <v>11</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="I35" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="L35" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>8</v>
@@ -1889,651 +1940,647 @@
       <c r="E36" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F36" s="3"/>
+      <c r="F36" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>161</v>
+      </c>
       <c r="L36" t="s">
-        <v>169</v>
+        <v>221</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
+      <c r="C37" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="F37" s="3"/>
-      <c r="H37" s="8" t="s">
-        <v>157</v>
-      </c>
       <c r="L37" t="s">
-        <v>170</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
-      <c r="C38" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="I38" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>171</v>
+      <c r="H38" s="8" t="s">
+        <v>151</v>
       </c>
       <c r="L38" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="27" x14ac:dyDescent="0.15">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="C39" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>8</v>
+        <v>105</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>109</v>
-      </c>
+      <c r="F39" s="3"/>
       <c r="I39" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="K39" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="L39" t="s">
         <v>167</v>
       </c>
-      <c r="L39" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A40" s="3" t="s">
+    </row>
+    <row r="40" spans="1:12" ht="27" x14ac:dyDescent="0.15">
+      <c r="A40" s="3"/>
+      <c r="C40" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="I40" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="L40" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A41" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" s="3"/>
-      <c r="H40" t="s">
-        <v>116</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="K40" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="L40" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A41" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F41" s="3"/>
       <c r="H41" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="L41" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.15">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A42" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F42" s="3"/>
       <c r="H42" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="K42" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="L42" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A43" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="H43" t="s">
+        <v>125</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="L43" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="L44" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A45" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="3"/>
+      <c r="H45" t="s">
+        <v>122</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="L45" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" s="3"/>
+      <c r="L46" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A47" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="H47" t="s">
+        <v>121</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="L47" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F48" s="3"/>
+      <c r="L48" t="s">
         <v>175</v>
       </c>
-      <c r="L42" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3" t="s">
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A49" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="3"/>
+      <c r="H49" t="s">
+        <v>119</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="L49" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="3" t="s">
+      <c r="D50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F43" s="3"/>
-      <c r="L43" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A44" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" s="3"/>
-      <c r="H44" t="s">
-        <v>124</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="L44" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F45" s="3"/>
-      <c r="L45" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A46" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F46" s="3"/>
-      <c r="H46" t="s">
-        <v>123</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="K46" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="L46" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F47" s="3"/>
-      <c r="L47" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A48" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F48" s="3"/>
-      <c r="H48" t="s">
-        <v>121</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="K48" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="L48" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F49" s="3"/>
-      <c r="L49" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A50" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F50" s="3"/>
-      <c r="H50" t="s">
-        <v>129</v>
-      </c>
-      <c r="I50" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="K50" s="4" t="s">
-        <v>167</v>
-      </c>
       <c r="L50" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A51" s="3" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+      <c r="D51" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E51" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F51" s="3"/>
+      <c r="H51" t="s">
+        <v>127</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="L51" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A52" s="3" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F52" s="3"/>
-      <c r="H52" t="s">
-        <v>131</v>
-      </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A53" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C53" s="3"/>
-      <c r="D53" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="F53" s="3"/>
-      <c r="I53" t="s">
-        <v>132</v>
-      </c>
-      <c r="J53" t="s">
-        <v>191</v>
-      </c>
-      <c r="K53" t="s">
-        <v>150</v>
-      </c>
-      <c r="L53" t="s">
-        <v>186</v>
+      <c r="H53" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A54" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
-      <c r="I54" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="J54" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="K54" s="8" t="s">
-        <v>188</v>
+      <c r="I54" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J54" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="K54" t="s">
+        <v>147</v>
       </c>
       <c r="L54" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="I55" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="J55" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="K55" t="s">
-        <v>158</v>
+        <v>130</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="K55" s="8" t="s">
+        <v>179</v>
       </c>
       <c r="L55" t="s">
-        <v>139</v>
+        <v>178</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A56" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F56" s="3"/>
-      <c r="I56" t="s">
-        <v>140</v>
+      <c r="I56" s="8" t="s">
+        <v>135</v>
       </c>
       <c r="J56" s="11" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="K56" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="L56" t="s">
-        <v>193</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A57" s="3" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
+      <c r="D57" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E57" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F57" s="3"/>
-      <c r="H57" t="s">
-        <v>141</v>
+      <c r="I57" t="s">
+        <v>137</v>
+      </c>
+      <c r="J57" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="K57" t="s">
+        <v>161</v>
+      </c>
+      <c r="L57" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A58" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C58" s="3"/>
-      <c r="D58" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="F58" s="3"/>
-      <c r="I58" t="s">
-        <v>142</v>
-      </c>
-      <c r="J58" t="s">
-        <v>195</v>
-      </c>
-      <c r="K58" t="s">
-        <v>150</v>
-      </c>
-      <c r="L58" t="s">
-        <v>194</v>
+      <c r="H58" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A59" s="3" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="D59" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="3"/>
       <c r="F59" s="3"/>
-      <c r="H59" t="s">
-        <v>143</v>
+      <c r="I59" t="s">
+        <v>139</v>
+      </c>
+      <c r="J59" t="s">
+        <v>185</v>
+      </c>
+      <c r="K59" t="s">
+        <v>147</v>
+      </c>
+      <c r="L59" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A60" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C60" s="3"/>
-      <c r="D60" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="F60" s="3"/>
-      <c r="I60" t="s">
-        <v>144</v>
-      </c>
-      <c r="J60" t="s">
-        <v>198</v>
-      </c>
-      <c r="K60" t="s">
-        <v>150</v>
-      </c>
-      <c r="L60" t="s">
-        <v>196</v>
+      <c r="H60" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A61" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E61" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="I61" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="J61" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="K61" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="L61" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A62" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F62" s="3"/>
-      <c r="H62" t="s">
-        <v>146</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="J62" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="K62" s="4" t="s">
-        <v>167</v>
+      <c r="I62" t="s">
+        <v>142</v>
+      </c>
+      <c r="J62" t="s">
+        <v>189</v>
+      </c>
+      <c r="K62" t="s">
+        <v>147</v>
       </c>
       <c r="L62" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A63" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
@@ -2544,45 +2591,76 @@
       </c>
       <c r="F63" s="3"/>
       <c r="H63" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="K63" s="4" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="L63" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B65" s="10" t="s">
-        <v>134</v>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A64" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" s="3"/>
+      <c r="H64" t="s">
+        <v>138</v>
+      </c>
+      <c r="I64" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J64" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="K64" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="L64" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B66" s="4" t="s">
-        <v>135</v>
+      <c r="B66" s="10" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B67" t="b">
-        <v>1</v>
-      </c>
-      <c r="C67" t="s">
-        <v>136</v>
+      <c r="B67" s="4" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B68" t="b">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B69" t="b">
         <v>0</v>
       </c>
-      <c r="C68" t="s">
-        <v>137</v>
+      <c r="C69" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>